<commit_message>
added lifetimes to ships
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -678,23 +678,23 @@
       </c>
       <c r="J14">
         <f ca="1">+RANDBETWEEN(1,9)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="K14">
         <f ca="1">+RANDBETWEEN(1,9)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L14">
         <f ca="1">+RANDBETWEEN(1,9)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M14">
         <f t="shared" ref="M14:N14" ca="1" si="0">+RANDBETWEEN(1,9)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="3:14">
@@ -711,15 +711,15 @@
       </c>
       <c r="J15">
         <f t="shared" ref="J15:N58" ca="1" si="3">+RANDBETWEEN(1,9)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M15">
         <f t="shared" ca="1" si="3"/>
@@ -727,7 +727,7 @@
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="3:14">
@@ -744,11 +744,11 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="3"/>
@@ -756,11 +756,11 @@
       </c>
       <c r="M16">
         <f t="shared" ca="1" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="N16">
+        <f t="shared" ca="1" si="3"/>
         <v>4</v>
-      </c>
-      <c r="N16">
-        <f t="shared" ca="1" si="3"/>
-        <v>5</v>
       </c>
     </row>
     <row r="17" spans="6:14">
@@ -777,19 +777,19 @@
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L17">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M17">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N17">
         <f t="shared" ca="1" si="3"/>
@@ -810,23 +810,23 @@
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="L18">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M18">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N18">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="6:14">
@@ -847,19 +847,19 @@
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="L19">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M19">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N19">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="6:14">
@@ -876,23 +876,23 @@
       </c>
       <c r="J20">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="K20">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L20">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M20">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N20">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="6:14">
@@ -909,7 +909,7 @@
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K21">
         <f t="shared" ca="1" si="3"/>
@@ -917,7 +917,7 @@
       </c>
       <c r="L21">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M21">
         <f t="shared" ca="1" si="3"/>
@@ -942,23 +942,23 @@
       </c>
       <c r="J22">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="K22">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L22">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M22">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N22">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="6:14">
@@ -975,19 +975,19 @@
       </c>
       <c r="J23">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K23">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L23">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M23">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N23">
         <f t="shared" ca="1" si="3"/>
@@ -1012,11 +1012,11 @@
       </c>
       <c r="K24">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L24">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M24">
         <f t="shared" ca="1" si="3"/>
@@ -1024,7 +1024,7 @@
       </c>
       <c r="N24">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="6:14">
@@ -1041,11 +1041,11 @@
       </c>
       <c r="J25">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K25">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L25">
         <f t="shared" ca="1" si="3"/>
@@ -1053,11 +1053,11 @@
       </c>
       <c r="M25">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="N25">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="6:14">
@@ -1074,23 +1074,23 @@
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="K26">
+        <f t="shared" ca="1" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="L26">
+        <f t="shared" ca="1" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="M26">
+        <f t="shared" ca="1" si="3"/>
         <v>6</v>
       </c>
-      <c r="K26">
-        <f t="shared" ca="1" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="L26">
-        <f t="shared" ca="1" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="M26">
-        <f t="shared" ca="1" si="3"/>
-        <v>3</v>
-      </c>
       <c r="N26">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="6:14">
@@ -1107,23 +1107,23 @@
       </c>
       <c r="J27">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K27">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L27">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M27">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N27">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="6:14">
@@ -1140,23 +1140,23 @@
       </c>
       <c r="J28">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K28">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L28">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="M28">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="N28">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="6:14">
@@ -1185,11 +1185,11 @@
       </c>
       <c r="M29">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N29">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="6:14">
@@ -1206,7 +1206,7 @@
       </c>
       <c r="J30">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K30">
         <f t="shared" ca="1" si="3"/>
@@ -1214,15 +1214,15 @@
       </c>
       <c r="L30">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M30">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="N30">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="6:14">
@@ -1239,23 +1239,23 @@
       </c>
       <c r="J31">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K31">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L31">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M31">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N31">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="6:14">
@@ -1272,23 +1272,23 @@
       </c>
       <c r="J32">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K32">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="L32">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M32">
         <f t="shared" ca="1" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="N32">
+        <f t="shared" ca="1" si="3"/>
         <v>8</v>
-      </c>
-      <c r="N32">
-        <f t="shared" ca="1" si="3"/>
-        <v>5</v>
       </c>
     </row>
     <row r="33" spans="6:14">
@@ -1309,19 +1309,19 @@
       </c>
       <c r="K33">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="L33">
         <f t="shared" ca="1" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="M33">
+        <f t="shared" ca="1" si="3"/>
         <v>5</v>
       </c>
-      <c r="M33">
+      <c r="N33">
         <f t="shared" ca="1" si="3"/>
         <v>4</v>
-      </c>
-      <c r="N33">
-        <f t="shared" ca="1" si="3"/>
-        <v>8</v>
       </c>
     </row>
     <row r="34" spans="6:14">
@@ -1338,23 +1338,23 @@
       </c>
       <c r="J34">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K34">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="L34">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M34">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="N34">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="6:14">
@@ -1371,19 +1371,19 @@
       </c>
       <c r="J35">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K35">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="L35">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M35">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="N35">
         <f t="shared" ca="1" si="3"/>
@@ -1404,23 +1404,23 @@
       </c>
       <c r="J36">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K36">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L36">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M36">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N36">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="6:14">
@@ -1437,23 +1437,23 @@
       </c>
       <c r="J37">
         <f t="shared" ca="1" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="K37">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <f t="shared" ca="1" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="M37">
+        <f t="shared" ca="1" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="N37">
+        <f t="shared" ca="1" si="3"/>
         <v>4</v>
-      </c>
-      <c r="K37">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L37">
-        <f t="shared" ca="1" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="M37">
-        <f t="shared" ca="1" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="N37">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
       </c>
     </row>
     <row r="38" spans="6:14">
@@ -1470,23 +1470,23 @@
       </c>
       <c r="J38">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="K38">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L38">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="M38">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="N38">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="6:14">
@@ -1503,7 +1503,7 @@
       </c>
       <c r="J39">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K39">
         <f t="shared" ca="1" si="3"/>
@@ -1511,15 +1511,15 @@
       </c>
       <c r="L39">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M39">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N39">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="6:14">
@@ -1540,19 +1540,19 @@
       </c>
       <c r="K40">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L40">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M40">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N40">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="6:14">
@@ -1569,23 +1569,23 @@
       </c>
       <c r="J41">
         <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="K41">
+        <f t="shared" ca="1" si="3"/>
         <v>7</v>
       </c>
-      <c r="K41">
-        <f t="shared" ca="1" si="3"/>
-        <v>4</v>
-      </c>
       <c r="L41">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="M41">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="N41">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="6:14">
@@ -1602,23 +1602,23 @@
       </c>
       <c r="J42">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K42">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L42">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="M42">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N42">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="6:14">
@@ -1635,23 +1635,23 @@
       </c>
       <c r="J43">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K43">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="L43">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="M43">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="N43">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="6:14">
@@ -1668,15 +1668,15 @@
       </c>
       <c r="J44">
         <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="K44">
+        <f t="shared" ca="1" si="3"/>
         <v>6</v>
       </c>
-      <c r="K44">
-        <f t="shared" ca="1" si="3"/>
-        <v>3</v>
-      </c>
       <c r="L44">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M44">
         <f t="shared" ca="1" si="3"/>
@@ -1684,7 +1684,7 @@
       </c>
       <c r="N44">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="6:14">
@@ -1701,23 +1701,23 @@
       </c>
       <c r="J45">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K45">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L45">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M45">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="N45">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="6:14">
@@ -1734,19 +1734,19 @@
       </c>
       <c r="J46">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="K46">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L46">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M46">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="N46">
         <f t="shared" ca="1" si="3"/>
@@ -1767,11 +1767,11 @@
       </c>
       <c r="J47">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K47">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="L47">
         <f t="shared" ca="1" si="3"/>
@@ -1779,11 +1779,11 @@
       </c>
       <c r="M47">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="N47">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="6:14">
@@ -1800,23 +1800,23 @@
       </c>
       <c r="J48">
         <f t="shared" ca="1" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="K48">
+        <f t="shared" ca="1" si="3"/>
         <v>5</v>
       </c>
-      <c r="K48">
-        <f t="shared" ca="1" si="3"/>
-        <v>4</v>
-      </c>
       <c r="L48">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="M48">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N48">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="6:14">
@@ -1833,11 +1833,11 @@
       </c>
       <c r="J49">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K49">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="L49">
         <f t="shared" ca="1" si="3"/>
@@ -1849,7 +1849,7 @@
       </c>
       <c r="N49">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="6:14">
@@ -1866,7 +1866,7 @@
       </c>
       <c r="J50">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K50">
         <f t="shared" ca="1" si="3"/>
@@ -1878,11 +1878,11 @@
       </c>
       <c r="M50">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N50">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="6:14">
@@ -1899,23 +1899,23 @@
       </c>
       <c r="J51">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K51">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L51">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M51">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N51">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="6:14">
@@ -1936,15 +1936,15 @@
       </c>
       <c r="K52">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L52">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M52">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N52">
         <f t="shared" ca="1" si="3"/>
@@ -1969,19 +1969,19 @@
       </c>
       <c r="K53">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L53">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M53">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="N53">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="6:14">
@@ -1998,23 +1998,23 @@
       </c>
       <c r="J54">
         <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="K54">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L54">
+        <f t="shared" ca="1" si="3"/>
         <v>6</v>
       </c>
-      <c r="K54">
-        <f t="shared" ca="1" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="L54">
+      <c r="M54">
         <f t="shared" ca="1" si="3"/>
         <v>9</v>
       </c>
-      <c r="M54">
-        <f t="shared" ca="1" si="3"/>
-        <v>8</v>
-      </c>
       <c r="N54">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="6:14">
@@ -2035,19 +2035,19 @@
       </c>
       <c r="K55">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L55">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="M55">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="N55">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="6:14">
@@ -2064,7 +2064,7 @@
       </c>
       <c r="J56">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K56">
         <f t="shared" ca="1" si="3"/>
@@ -2072,7 +2072,7 @@
       </c>
       <c r="L56">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="M56">
         <f t="shared" ca="1" si="3"/>
@@ -2080,7 +2080,7 @@
       </c>
       <c r="N56">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="6:14">
@@ -2097,23 +2097,23 @@
       </c>
       <c r="J57">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="K57">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="L57">
         <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="M57">
+        <f t="shared" ca="1" si="3"/>
         <v>6</v>
       </c>
-      <c r="M57">
-        <f t="shared" ca="1" si="3"/>
-        <v>2</v>
-      </c>
       <c r="N57">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="6:14">
@@ -2130,23 +2130,23 @@
       </c>
       <c r="J58">
         <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="K58">
+        <f t="shared" ca="1" si="3"/>
         <v>7</v>
       </c>
-      <c r="K58">
-        <f t="shared" ca="1" si="3"/>
-        <v>7</v>
-      </c>
       <c r="L58">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M58">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="N58">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2158,8 +2158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:H43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2180,7 +2180,7 @@
         <v>2011</v>
       </c>
       <c r="D4" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F4" s="2">
         <v>1000000</v>
@@ -2202,7 +2202,7 @@
         <v>2012</v>
       </c>
       <c r="D5" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F5" s="2">
         <v>1000000</v>
@@ -2224,7 +2224,7 @@
         <v>2013</v>
       </c>
       <c r="D6" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F6" s="2">
         <v>1000000</v>
@@ -2246,7 +2246,7 @@
         <v>2014</v>
       </c>
       <c r="D7" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F7" s="2">
         <v>1000000</v>
@@ -2268,7 +2268,7 @@
         <v>2015</v>
       </c>
       <c r="D8" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F8" s="2">
         <v>1000000</v>
@@ -2290,7 +2290,7 @@
         <v>2016</v>
       </c>
       <c r="D9" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F9" s="2">
         <v>1000000</v>
@@ -2312,7 +2312,7 @@
         <v>2017</v>
       </c>
       <c r="D10" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F10" s="2">
         <v>1000000</v>
@@ -2334,7 +2334,7 @@
         <v>2018</v>
       </c>
       <c r="D11" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F11" s="2">
         <v>1000000</v>
@@ -2356,7 +2356,7 @@
         <v>2019</v>
       </c>
       <c r="D12" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F12" s="2">
         <v>1000000</v>
@@ -2378,7 +2378,7 @@
         <v>2020</v>
       </c>
       <c r="D13" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F13" s="2">
         <v>1000000</v>
@@ -2400,7 +2400,7 @@
         <v>2021</v>
       </c>
       <c r="D14" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F14" s="2">
         <v>1000000</v>
@@ -2422,7 +2422,7 @@
         <v>2022</v>
       </c>
       <c r="D15" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F15" s="2">
         <v>1000000</v>
@@ -2444,7 +2444,7 @@
         <v>2023</v>
       </c>
       <c r="D16" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F16" s="2">
         <v>1000000</v>
@@ -2466,7 +2466,7 @@
         <v>2024</v>
       </c>
       <c r="D17" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F17" s="2">
         <v>1000000</v>
@@ -2488,7 +2488,7 @@
         <v>2025</v>
       </c>
       <c r="D18" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F18" s="2">
         <v>1000000</v>
@@ -2510,7 +2510,7 @@
         <v>2026</v>
       </c>
       <c r="D19" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F19" s="2">
         <v>1000000</v>
@@ -2532,7 +2532,7 @@
         <v>2027</v>
       </c>
       <c r="D20" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F20" s="2">
         <v>1000000</v>
@@ -2554,7 +2554,7 @@
         <v>2028</v>
       </c>
       <c r="D21" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F21" s="2">
         <v>1000000</v>
@@ -2576,7 +2576,7 @@
         <v>2029</v>
       </c>
       <c r="D22" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F22" s="2">
         <v>1000000</v>
@@ -2598,7 +2598,7 @@
         <v>2030</v>
       </c>
       <c r="D23" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F23" s="2">
         <v>1000000</v>
@@ -2620,7 +2620,7 @@
         <v>2031</v>
       </c>
       <c r="D24" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F24" s="2">
         <v>1000000</v>
@@ -2642,7 +2642,7 @@
         <v>2032</v>
       </c>
       <c r="D25" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F25" s="2">
         <v>1000000</v>
@@ -2664,7 +2664,7 @@
         <v>2033</v>
       </c>
       <c r="D26" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F26" s="2">
         <v>1000000</v>
@@ -2686,7 +2686,7 @@
         <v>2034</v>
       </c>
       <c r="D27" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F27" s="2">
         <v>1000000</v>
@@ -2708,7 +2708,7 @@
         <v>2035</v>
       </c>
       <c r="D28" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F28" s="2">
         <v>1000000</v>
@@ -2730,7 +2730,7 @@
         <v>2036</v>
       </c>
       <c r="D29" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F29" s="2">
         <v>1000000</v>
@@ -2752,7 +2752,7 @@
         <v>2037</v>
       </c>
       <c r="D30" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F30" s="2">
         <v>1000000</v>
@@ -2774,7 +2774,7 @@
         <v>2038</v>
       </c>
       <c r="D31" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F31" s="2">
         <v>1000000</v>
@@ -2796,7 +2796,7 @@
         <v>2039</v>
       </c>
       <c r="D32" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F32" s="2">
         <v>1000000</v>
@@ -2818,7 +2818,7 @@
         <v>2040</v>
       </c>
       <c r="D33" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F33" s="2">
         <v>1000000</v>
@@ -2840,7 +2840,7 @@
         <v>2041</v>
       </c>
       <c r="D34" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F34" s="2">
         <v>1000000</v>
@@ -2862,7 +2862,7 @@
         <v>2042</v>
       </c>
       <c r="D35" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F35" s="2">
         <v>1000000</v>
@@ -2884,7 +2884,7 @@
         <v>2043</v>
       </c>
       <c r="D36" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F36" s="2">
         <v>1000000</v>
@@ -2906,7 +2906,7 @@
         <v>2044</v>
       </c>
       <c r="D37" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F37" s="2">
         <v>1000000</v>
@@ -2928,7 +2928,7 @@
         <v>2045</v>
       </c>
       <c r="D38" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F38" s="2">
         <v>1000000</v>
@@ -2950,7 +2950,7 @@
         <v>2046</v>
       </c>
       <c r="D39" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F39" s="2">
         <v>1000000</v>
@@ -2972,7 +2972,7 @@
         <v>2047</v>
       </c>
       <c r="D40" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F40" s="2">
         <v>1000000</v>
@@ -2994,7 +2994,7 @@
         <v>2048</v>
       </c>
       <c r="D41" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F41" s="2">
         <v>1000000</v>
@@ -3016,7 +3016,7 @@
         <v>2049</v>
       </c>
       <c r="D42" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F42" s="2">
         <v>1000000</v>
@@ -3038,7 +3038,7 @@
         <v>2050</v>
       </c>
       <c r="D43" s="1">
-        <v>700000</v>
+        <v>7000000</v>
       </c>
       <c r="F43" s="2">
         <v>1000000</v>
@@ -9045,7 +9045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add merchant fleet data and existing fleet data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="77">
   <si>
     <t>_</t>
   </si>
@@ -239,6 +239,27 @@
   <si>
     <t>p86 of Maritime Forecast to 2050</t>
   </si>
+  <si>
+    <t>Total fleet</t>
+  </si>
+  <si>
+    <t>Oil tankers</t>
+  </si>
+  <si>
+    <t>Bulk carriers</t>
+  </si>
+  <si>
+    <t>General cargo</t>
+  </si>
+  <si>
+    <t>Container ships</t>
+  </si>
+  <si>
+    <t>Other types of ships</t>
+  </si>
+  <si>
+    <t># of ships</t>
+  </si>
 </sst>
 </file>
 
@@ -270,10 +291,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1184,12 +1206,252 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C1:L8"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:12">
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="3:12">
+      <c r="D2">
+        <v>2011</v>
+      </c>
+      <c r="E2">
+        <f>+D2+1</f>
+        <v>2012</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:L2" si="0">+E2+1</f>
+        <v>2013</v>
+      </c>
+      <c r="G2">
+        <f t="shared" si="0"/>
+        <v>2014</v>
+      </c>
+      <c r="H2">
+        <f t="shared" si="0"/>
+        <v>2015</v>
+      </c>
+      <c r="I2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="J2">
+        <f t="shared" si="0"/>
+        <v>2017</v>
+      </c>
+      <c r="K2">
+        <f t="shared" si="0"/>
+        <v>2018</v>
+      </c>
+      <c r="L2">
+        <f t="shared" si="0"/>
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="3" spans="3:12">
+      <c r="C3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="3">
+        <v>83283</v>
+      </c>
+      <c r="E3" s="3">
+        <v>84709</v>
+      </c>
+      <c r="F3" s="3">
+        <v>86484</v>
+      </c>
+      <c r="G3" s="3">
+        <v>87954</v>
+      </c>
+      <c r="H3" s="3">
+        <v>90470</v>
+      </c>
+      <c r="I3" s="3">
+        <v>92074</v>
+      </c>
+      <c r="J3" s="3">
+        <v>93262</v>
+      </c>
+      <c r="K3" s="3">
+        <v>94169</v>
+      </c>
+      <c r="L3" s="3">
+        <v>96295</v>
+      </c>
+    </row>
+    <row r="4" spans="3:12">
+      <c r="C4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="3">
+        <v>10609</v>
+      </c>
+      <c r="E4" s="3">
+        <v>8838</v>
+      </c>
+      <c r="F4" s="3">
+        <v>9033</v>
+      </c>
+      <c r="G4" s="3">
+        <v>9241</v>
+      </c>
+      <c r="H4" s="3">
+        <v>9695</v>
+      </c>
+      <c r="I4" s="3">
+        <v>9935</v>
+      </c>
+      <c r="J4" s="3">
+        <v>10216</v>
+      </c>
+      <c r="K4" s="3">
+        <v>10420</v>
+      </c>
+      <c r="L4" s="3">
+        <v>10766</v>
+      </c>
+    </row>
+    <row r="5" spans="3:12">
+      <c r="C5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="3">
+        <v>8228</v>
+      </c>
+      <c r="E5" s="3">
+        <v>9001</v>
+      </c>
+      <c r="F5" s="3">
+        <v>9568</v>
+      </c>
+      <c r="G5" s="3">
+        <v>10162</v>
+      </c>
+      <c r="H5" s="3">
+        <v>10509</v>
+      </c>
+      <c r="I5" s="3">
+        <v>10747</v>
+      </c>
+      <c r="J5" s="3">
+        <v>10892</v>
+      </c>
+      <c r="K5" s="3">
+        <v>11125</v>
+      </c>
+      <c r="L5" s="3">
+        <v>11373</v>
+      </c>
+    </row>
+    <row r="6" spans="3:12">
+      <c r="C6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="3">
+        <v>21090</v>
+      </c>
+      <c r="E6" s="3">
+        <v>20309</v>
+      </c>
+      <c r="F6" s="3">
+        <v>20282</v>
+      </c>
+      <c r="G6" s="3">
+        <v>19664</v>
+      </c>
+      <c r="H6" s="3">
+        <v>19566</v>
+      </c>
+      <c r="I6" s="3">
+        <v>19698</v>
+      </c>
+      <c r="J6" s="3">
+        <v>19716</v>
+      </c>
+      <c r="K6" s="3">
+        <v>19613</v>
+      </c>
+      <c r="L6" s="3">
+        <v>18993</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12">
+      <c r="C7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="3">
+        <v>4966</v>
+      </c>
+      <c r="E7" s="3">
+        <v>5096</v>
+      </c>
+      <c r="F7" s="3">
+        <v>5107</v>
+      </c>
+      <c r="G7" s="3">
+        <v>5101</v>
+      </c>
+      <c r="H7" s="3">
+        <v>5111</v>
+      </c>
+      <c r="I7" s="3">
+        <v>5227</v>
+      </c>
+      <c r="J7" s="3">
+        <v>5158</v>
+      </c>
+      <c r="K7" s="3">
+        <v>5164</v>
+      </c>
+      <c r="L7" s="3">
+        <v>5269</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12">
+      <c r="C8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="3">
+        <v>38390</v>
+      </c>
+      <c r="E8" s="3">
+        <v>41465</v>
+      </c>
+      <c r="F8" s="3">
+        <v>42494</v>
+      </c>
+      <c r="G8" s="3">
+        <v>43786</v>
+      </c>
+      <c r="H8" s="3">
+        <v>45589</v>
+      </c>
+      <c r="I8" s="3">
+        <v>46467</v>
+      </c>
+      <c r="J8" s="3">
+        <v>47280</v>
+      </c>
+      <c r="K8" s="3">
+        <v>47847</v>
+      </c>
+      <c r="L8" s="3">
+        <v>49894</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5994,7 +6256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AD47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E5" workbookViewId="0">
+    <sheetView topLeftCell="E5" workbookViewId="0">
       <selection activeCell="AD47" sqref="S8:AD47"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
changes to code where fuel and ships are split and ships can choose fuel
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -22,13 +22,14 @@
     <sheet name="ship_inv" sheetId="9" r:id="rId8"/>
     <sheet name="Demand forecasts" sheetId="11" r:id="rId9"/>
     <sheet name="Preexisting fleet" sheetId="12" r:id="rId10"/>
+    <sheet name="Sheet6" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="80">
   <si>
     <t>_</t>
   </si>
@@ -259,6 +260,15 @@
   </si>
   <si>
     <t># of ships</t>
+  </si>
+  <si>
+    <t>MFO</t>
+  </si>
+  <si>
+    <t>ammonia</t>
+  </si>
+  <si>
+    <t>methanol</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1218,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1449,6 +1459,671 @@
       </c>
       <c r="L8" s="3">
         <v>49894</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A5:AO16"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U28" sqref="U27:U28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5" spans="1:41">
+      <c r="B5">
+        <v>2011</v>
+      </c>
+      <c r="C5">
+        <f>+B5+1</f>
+        <v>2012</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:AO5" si="0">+C5+1</f>
+        <v>2013</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>2014</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>2015</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>2017</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>2018</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>2019</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>2020</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>2021</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>2022</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>2023</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>2025</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>2026</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="0"/>
+        <v>2027</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="0"/>
+        <v>2028</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="0"/>
+        <v>2029</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="0"/>
+        <v>2030</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="0"/>
+        <v>2031</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="0"/>
+        <v>2032</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="0"/>
+        <v>2033</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="0"/>
+        <v>2034</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="0"/>
+        <v>2035</v>
+      </c>
+      <c r="AA5">
+        <f t="shared" si="0"/>
+        <v>2036</v>
+      </c>
+      <c r="AB5">
+        <f t="shared" si="0"/>
+        <v>2037</v>
+      </c>
+      <c r="AC5">
+        <f t="shared" si="0"/>
+        <v>2038</v>
+      </c>
+      <c r="AD5">
+        <f t="shared" si="0"/>
+        <v>2039</v>
+      </c>
+      <c r="AE5">
+        <f t="shared" si="0"/>
+        <v>2040</v>
+      </c>
+      <c r="AF5">
+        <f t="shared" si="0"/>
+        <v>2041</v>
+      </c>
+      <c r="AG5">
+        <f t="shared" si="0"/>
+        <v>2042</v>
+      </c>
+      <c r="AH5">
+        <f t="shared" si="0"/>
+        <v>2043</v>
+      </c>
+      <c r="AI5">
+        <f t="shared" si="0"/>
+        <v>2044</v>
+      </c>
+      <c r="AJ5">
+        <f>+AI5+1</f>
+        <v>2045</v>
+      </c>
+      <c r="AK5">
+        <f t="shared" si="0"/>
+        <v>2046</v>
+      </c>
+      <c r="AL5">
+        <f t="shared" si="0"/>
+        <v>2047</v>
+      </c>
+      <c r="AM5">
+        <f t="shared" si="0"/>
+        <v>2048</v>
+      </c>
+      <c r="AN5">
+        <f t="shared" si="0"/>
+        <v>2049</v>
+      </c>
+      <c r="AO5">
+        <f t="shared" si="0"/>
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41">
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6">
+        <v>1</v>
+      </c>
+      <c r="AC6">
+        <v>1</v>
+      </c>
+      <c r="AD6">
+        <v>1</v>
+      </c>
+      <c r="AE6">
+        <v>1</v>
+      </c>
+      <c r="AF6">
+        <v>1</v>
+      </c>
+      <c r="AG6">
+        <v>1</v>
+      </c>
+      <c r="AH6">
+        <v>1</v>
+      </c>
+      <c r="AI6">
+        <v>1</v>
+      </c>
+      <c r="AJ6">
+        <v>1</v>
+      </c>
+      <c r="AK6">
+        <v>1</v>
+      </c>
+      <c r="AL6">
+        <v>1</v>
+      </c>
+      <c r="AM6">
+        <v>1</v>
+      </c>
+      <c r="AN6">
+        <v>1</v>
+      </c>
+      <c r="AO6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41">
+      <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7">
+        <v>1</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>1</v>
+      </c>
+      <c r="Y7">
+        <v>1</v>
+      </c>
+      <c r="Z7">
+        <v>1</v>
+      </c>
+      <c r="AA7">
+        <v>1</v>
+      </c>
+      <c r="AB7">
+        <v>1</v>
+      </c>
+      <c r="AC7">
+        <v>1</v>
+      </c>
+      <c r="AD7">
+        <v>1</v>
+      </c>
+      <c r="AE7">
+        <v>1</v>
+      </c>
+      <c r="AF7">
+        <v>1</v>
+      </c>
+      <c r="AG7">
+        <v>1</v>
+      </c>
+      <c r="AH7">
+        <v>1</v>
+      </c>
+      <c r="AI7">
+        <v>1</v>
+      </c>
+      <c r="AJ7">
+        <v>1</v>
+      </c>
+      <c r="AK7">
+        <v>1</v>
+      </c>
+      <c r="AL7">
+        <v>1</v>
+      </c>
+      <c r="AM7">
+        <v>1</v>
+      </c>
+      <c r="AN7">
+        <v>1</v>
+      </c>
+      <c r="AO7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41">
+      <c r="A8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="Z8">
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <v>1</v>
+      </c>
+      <c r="AB8">
+        <v>1</v>
+      </c>
+      <c r="AC8">
+        <v>1</v>
+      </c>
+      <c r="AD8">
+        <v>1</v>
+      </c>
+      <c r="AE8">
+        <v>1</v>
+      </c>
+      <c r="AF8">
+        <v>1</v>
+      </c>
+      <c r="AG8">
+        <v>1</v>
+      </c>
+      <c r="AH8">
+        <v>1</v>
+      </c>
+      <c r="AI8">
+        <v>1</v>
+      </c>
+      <c r="AJ8">
+        <v>1</v>
+      </c>
+      <c r="AK8">
+        <v>1</v>
+      </c>
+      <c r="AL8">
+        <v>1</v>
+      </c>
+      <c r="AM8">
+        <v>1</v>
+      </c>
+      <c r="AN8">
+        <v>1</v>
+      </c>
+      <c r="AO8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41">
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41">
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2001,8 +2676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B13:AP61"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:E61"/>
+    <sheetView topLeftCell="O10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:AP13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11611,8 +12286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11655,19 +12330,19 @@
         <v>2011</v>
       </c>
       <c r="D7" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E7" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F7" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G7" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H7" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="8" spans="2:8">
@@ -11676,19 +12351,19 @@
         <v>2012</v>
       </c>
       <c r="D8" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E8" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F8" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G8" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H8" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="9" spans="2:8">
@@ -11697,19 +12372,19 @@
         <v>2013</v>
       </c>
       <c r="D9" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E9" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F9" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G9" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H9" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="10" spans="2:8">
@@ -11718,19 +12393,19 @@
         <v>2014</v>
       </c>
       <c r="D10" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E10" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F10" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G10" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H10" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="11" spans="2:8">
@@ -11739,19 +12414,19 @@
         <v>2015</v>
       </c>
       <c r="D11" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E11" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F11" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G11" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H11" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="12" spans="2:8">
@@ -11760,19 +12435,19 @@
         <v>2016</v>
       </c>
       <c r="D12" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E12" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F12" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G12" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H12" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="13" spans="2:8">
@@ -11781,19 +12456,19 @@
         <v>2017</v>
       </c>
       <c r="D13" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E13" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F13" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G13" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H13" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="14" spans="2:8">
@@ -11802,19 +12477,19 @@
         <v>2018</v>
       </c>
       <c r="D14" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E14" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F14" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G14" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H14" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="15" spans="2:8">
@@ -11823,19 +12498,19 @@
         <v>2019</v>
       </c>
       <c r="D15" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E15" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F15" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G15" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H15" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="16" spans="2:8">
@@ -11844,19 +12519,19 @@
         <v>2020</v>
       </c>
       <c r="D16" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E16" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F16" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G16" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H16" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="17" spans="3:8">
@@ -11865,19 +12540,19 @@
         <v>2021</v>
       </c>
       <c r="D17" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E17" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F17" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G17" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H17" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="18" spans="3:8">
@@ -11886,19 +12561,19 @@
         <v>2022</v>
       </c>
       <c r="D18" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E18" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F18" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G18" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H18" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="19" spans="3:8">
@@ -11907,19 +12582,19 @@
         <v>2023</v>
       </c>
       <c r="D19" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E19" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F19" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G19" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H19" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="20" spans="3:8">
@@ -11928,19 +12603,19 @@
         <v>2024</v>
       </c>
       <c r="D20" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E20" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F20" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G20" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H20" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="21" spans="3:8">
@@ -11949,19 +12624,19 @@
         <v>2025</v>
       </c>
       <c r="D21" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E21" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F21" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G21" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H21" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="22" spans="3:8">
@@ -11970,19 +12645,19 @@
         <v>2026</v>
       </c>
       <c r="D22" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E22" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F22" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G22" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H22" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="23" spans="3:8">
@@ -11991,19 +12666,19 @@
         <v>2027</v>
       </c>
       <c r="D23" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E23" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F23" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G23" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H23" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="24" spans="3:8">
@@ -12012,19 +12687,19 @@
         <v>2028</v>
       </c>
       <c r="D24" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E24" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F24" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G24" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H24" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="25" spans="3:8">
@@ -12033,19 +12708,19 @@
         <v>2029</v>
       </c>
       <c r="D25" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E25" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F25" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G25" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H25" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="26" spans="3:8">
@@ -12054,19 +12729,19 @@
         <v>2030</v>
       </c>
       <c r="D26" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E26" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F26" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G26" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H26" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="27" spans="3:8">
@@ -12075,19 +12750,19 @@
         <v>2031</v>
       </c>
       <c r="D27" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E27" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F27" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G27" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H27" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="28" spans="3:8">
@@ -12096,19 +12771,19 @@
         <v>2032</v>
       </c>
       <c r="D28" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E28" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F28" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G28" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H28" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="29" spans="3:8">
@@ -12117,19 +12792,19 @@
         <v>2033</v>
       </c>
       <c r="D29" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E29" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F29" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G29" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H29" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="30" spans="3:8">
@@ -12138,19 +12813,19 @@
         <v>2034</v>
       </c>
       <c r="D30" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E30" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F30" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G30" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H30" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="31" spans="3:8">
@@ -12159,19 +12834,19 @@
         <v>2035</v>
       </c>
       <c r="D31" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E31" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F31" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G31" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H31" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="32" spans="3:8">
@@ -12180,19 +12855,19 @@
         <v>2036</v>
       </c>
       <c r="D32" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E32" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F32" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G32" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H32" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="33" spans="3:8">
@@ -12201,19 +12876,19 @@
         <v>2037</v>
       </c>
       <c r="D33" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E33" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F33" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G33" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H33" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="34" spans="3:8">
@@ -12222,19 +12897,19 @@
         <v>2038</v>
       </c>
       <c r="D34" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E34" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F34" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G34" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H34" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="35" spans="3:8">
@@ -12243,19 +12918,19 @@
         <v>2039</v>
       </c>
       <c r="D35" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E35" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F35" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G35" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H35" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="36" spans="3:8">
@@ -12264,19 +12939,19 @@
         <v>2040</v>
       </c>
       <c r="D36" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E36" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F36" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G36" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H36" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="37" spans="3:8">
@@ -12285,19 +12960,19 @@
         <v>2041</v>
       </c>
       <c r="D37" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E37" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F37" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G37" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H37" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="38" spans="3:8">
@@ -12306,19 +12981,19 @@
         <v>2042</v>
       </c>
       <c r="D38" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E38" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F38" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G38" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H38" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="39" spans="3:8">
@@ -12327,19 +13002,19 @@
         <v>2043</v>
       </c>
       <c r="D39" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E39" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F39" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G39" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H39" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="40" spans="3:8">
@@ -12348,19 +13023,19 @@
         <v>2044</v>
       </c>
       <c r="D40" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E40" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F40" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G40" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H40" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="41" spans="3:8">
@@ -12369,19 +13044,19 @@
         <v>2045</v>
       </c>
       <c r="D41" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E41" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F41" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G41" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H41" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="42" spans="3:8">
@@ -12390,19 +13065,19 @@
         <v>2046</v>
       </c>
       <c r="D42" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E42" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F42" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G42" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H42" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="43" spans="3:8">
@@ -12411,19 +13086,19 @@
         <v>2047</v>
       </c>
       <c r="D43" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E43" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F43" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G43" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H43" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="44" spans="3:8">
@@ -12432,19 +13107,19 @@
         <v>2048</v>
       </c>
       <c r="D44" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E44" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F44" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G44" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H44" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="45" spans="3:8">
@@ -12453,19 +13128,19 @@
         <v>2049</v>
       </c>
       <c r="D45" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E45" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F45" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G45" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H45" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="46" spans="3:8">
@@ -12474,19 +13149,19 @@
         <v>2050</v>
       </c>
       <c r="D46" s="2">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="E46" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="F46" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
       <c r="G46" s="2">
-        <v>4000000</v>
+        <v>500000</v>
       </c>
       <c r="H46" s="2">
-        <v>900000</v>
+        <v>500000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>